<commit_message>
Homework and lab updates.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE7B939-F402-A142-903E-D49E06B2C1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E171939D-F22B-A840-919A-4CE6375B62C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16040" yWindow="9660" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="1040" yWindow="1940" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -193,9 +193,6 @@
     <t>/static/homework/homework8.pdf</t>
   </si>
   <si>
-    <t>/static/homework/homework9.pdf</t>
-  </si>
-  <si>
     <t>/static/labs/02_intro_to_data.zip</t>
   </si>
   <si>
@@ -218,6 +215,15 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>/static/homework/homework9_mr.pdf</t>
+  </si>
+  <si>
+    <t>/static/homework/homework9_lr.pdf</t>
+  </si>
+  <si>
+    <t>/static/labs/09_logistic_regression.zip</t>
   </si>
 </sst>
 </file>
@@ -611,7 +617,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,7 +704,7 @@
         <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -721,7 +727,7 @@
         <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -744,7 +750,7 @@
         <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -767,7 +773,7 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -790,7 +796,7 @@
         <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -813,7 +819,7 @@
         <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -829,7 +835,12 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -848,10 +859,10 @@
         <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -874,7 +885,7 @@
         <v>45601</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added slides. Fixed names for labs.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9155559F-CA5D-0548-A3BA-F58628BF4FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406724C6-BCBB-1D4C-93E7-9F6CA7424F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="7780" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="4440" yWindow="7860" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -196,21 +196,6 @@
     <t>/static/labs/03_probability.zip</t>
   </si>
   <si>
-    <t>/static/labs/11_foundations_for_inference.zip</t>
-  </si>
-  <si>
-    <t>/static/labs/16_inference_for_categorial_data.zip</t>
-  </si>
-  <si>
-    <t>/static/labs/19_inference_for_numerical_data</t>
-  </si>
-  <si>
-    <t>/static/labs/07_simple_linear_regression.zip</t>
-  </si>
-  <si>
-    <t>/static/labs/08_multiple_regression.zip</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -230,6 +215,24 @@
   </si>
   <si>
     <t>7:30pm</t>
+  </si>
+  <si>
+    <t>/static/labs/05_foundations_for_inference.zip</t>
+  </si>
+  <si>
+    <t>/static/labs/06_inference_for_categorial_data.zip</t>
+  </si>
+  <si>
+    <t>/static/labs/07_inference_for_numerical_data</t>
+  </si>
+  <si>
+    <t>/static/labs/08_simple_linear_regression.zip</t>
+  </si>
+  <si>
+    <t>/static/labs/09_multiple_regression.zip</t>
+  </si>
+  <si>
+    <t>/slides/03-Probability_and_Distributions.html</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,7 +678,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -701,13 +704,13 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
         <v>45</v>
@@ -727,10 +730,13 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
       </c>
       <c r="G4" t="s">
         <v>46</v>
@@ -750,7 +756,7 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -759,7 +765,7 @@
         <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -773,7 +779,7 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -782,7 +788,7 @@
         <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -796,7 +802,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -805,7 +811,7 @@
         <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -819,7 +825,7 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
@@ -828,7 +834,7 @@
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -842,16 +848,16 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -865,16 +871,16 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -888,7 +894,7 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -897,13 +903,13 @@
         <v>45601</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -918,7 +924,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -933,7 +939,7 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -957,7 +963,7 @@
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -975,7 +981,7 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G17" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added link to slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CFADB1-709D-0948-BCB8-47F15F8EA58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18551971-CD01-6A4D-9C39-07C68D944511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17160" yWindow="8420" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>/static/labs/07_inference_for_numerical_data.zip</t>
+  </si>
+  <si>
+    <t>/slides/08-Linear_Regression.html</t>
   </si>
 </sst>
 </file>
@@ -635,7 +638,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,6 +850,9 @@
       </c>
       <c r="E8" t="s">
         <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Updated link for slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2024 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18551971-CD01-6A4D-9C39-07C68D944511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3715982-15D2-A248-A39A-624EC10C1E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="8420" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -238,13 +238,13 @@
     <t>/slides/06-Inference_for_Categorical_Data.html</t>
   </si>
   <si>
-    <t>/slides/06-Inference_for_Numerical_Data.html</t>
-  </si>
-  <si>
     <t>/static/labs/07_inference_for_numerical_data.zip</t>
   </si>
   <si>
     <t>/slides/08-Linear_Regression.html</t>
+  </si>
+  <si>
+    <t>/slides/07-Inference_for_Numerical_Data.html</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,13 +826,13 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
         <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -852,7 +852,7 @@
         <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>
@@ -965,6 +965,9 @@
       <c r="D14" t="s">
         <v>59</v>
       </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -988,9 +991,6 @@
       </c>
       <c r="D16" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" t="s">
-        <v>30</v>
       </c>
       <c r="G16" s="4"/>
     </row>

</xml_diff>